<commit_message>
COMBINE ab and cp
</commit_message>
<xml_diff>
--- a/source_code/data/results/[1_high_electricity_price]_#_fix_cost.xlsx
+++ b/source_code/data/results/[1_high_electricity_price]_#_fix_cost.xlsx
@@ -510,7 +510,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8095.925712661734</v>
+        <v>8095.925712661735</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8095.925712661734</v>
+        <v>8095.925712661735</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -716,7 +716,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8095.925712661734</v>
+        <v>8095.925712661735</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8095.925712661734</v>
+        <v>8095.925712661735</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -922,7 +922,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8095.925712661734</v>
+        <v>8095.925712661735</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -1025,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8095.925712661734</v>
+        <v>8095.925712661735</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>

</xml_diff>